<commit_message>
Amélioration du propagateur d'égalité.
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -70,6 +70,30 @@
   </si>
   <si>
     <t>Un premier algorihtme de propagation pour la contrainte allDifferent.</t>
+  </si>
+  <si>
+    <t>LCP-1</t>
+  </si>
+  <si>
+    <t>LCP-2</t>
+  </si>
+  <si>
+    <t>LCP-3</t>
+  </si>
+  <si>
+    <t>LCP-4</t>
+  </si>
+  <si>
+    <t>LCP-5</t>
+  </si>
+  <si>
+    <t>LCP-6</t>
+  </si>
+  <si>
+    <t>LCP-7</t>
+  </si>
+  <si>
+    <t>LCP-8</t>
   </si>
 </sst>
 </file>
@@ -192,18 +216,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -507,7 +524,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,8 +553,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>1</v>
+      <c r="A2" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>3</v>
@@ -553,8 +570,8 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
+      <c r="A3" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>4</v>
@@ -568,8 +585,8 @@
       <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
+      <c r="A4" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>17</v>
@@ -583,8 +600,8 @@
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>4</v>
+      <c r="A5" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>6</v>
@@ -598,8 +615,8 @@
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
+      <c r="A6" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>7</v>
@@ -613,8 +630,8 @@
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>6</v>
+      <c r="A7" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>8</v>
@@ -628,8 +645,8 @@
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>7</v>
+      <c r="A8" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>9</v>
@@ -643,8 +660,8 @@
       <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>8</v>
+      <c r="A9" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Une variable connait l'ensemble des constraintes dans laquelle elle est impliquée.
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$E$1</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>ID</t>
   </si>
@@ -94,6 +97,24 @@
   </si>
   <si>
     <t>LCP-8</t>
+  </si>
+  <si>
+    <t>LCP-9</t>
+  </si>
+  <si>
+    <t>Rechercher plusieurs solutions.</t>
+  </si>
+  <si>
+    <t>LCP-10</t>
+  </si>
+  <si>
+    <t>Rechercher la meilleur solution (fonction d'optimisation).</t>
+  </si>
+  <si>
+    <t>LCP-11</t>
+  </si>
+  <si>
+    <t>Ajout d'heuristique plus avancées (eg. DomOverWDeg).</t>
   </si>
 </sst>
 </file>
@@ -524,7 +545,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,19 +598,21 @@
         <v>4</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="10">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>11</v>
@@ -597,44 +620,50 @@
       <c r="D4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="10"/>
+      <c r="E4" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="E5" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="E6" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>11</v>
@@ -642,56 +671,94 @@
       <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="10"/>
+        <v>16</v>
+      </c>
+      <c r="E8" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="10"/>
+      <c r="D9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="10"/>
+      <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="10"/>
+      <c r="A11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="10"/>
+      <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="10">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
@@ -960,6 +1027,10 @@
       <c r="E50" s="10"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E1"/>
+  <sortState ref="A2:E12">
+    <sortCondition ref="E2:E12"/>
+  </sortState>
   <conditionalFormatting sqref="A2:E50">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)</formula>

</xml_diff>